<commit_message>
Updated the order form
</commit_message>
<xml_diff>
--- a/import/Spreadsheets/Order Form.xlsx
+++ b/import/Spreadsheets/Order Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Astrid Delestine\Real_Documents\GitStuff\Senior-Design-Capstone-25\import\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117E78F-BF5F-45E4-B2CA-A1BDF0DEDAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9AA7A9-727B-4E20-8614-97DFB2755251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
     <col min="7" max="7" width="120" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -578,7 +578,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -616,7 +616,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -692,7 +692,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -768,7 +768,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>22</v>
       </c>
@@ -823,7 +823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
@@ -837,7 +837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
@@ -851,7 +851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -865,7 +865,7 @@
         <v>-6.67</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
@@ -897,11 +897,15 @@
       <c r="A15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="13">
+        <v>1</v>
+      </c>
       <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="14">
+        <v>72.86</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="13"/>
@@ -1086,22 +1090,22 @@
       <c r="H32" s="17"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="12" cm="1">
         <f t="array" ref="B36" xml:space="preserve"> SUM(B2:B15*D2:D15)</f>
-        <v>286.74</v>
+        <v>359.6</v>
       </c>
       <c r="D36" s="12"/>
     </row>

</xml_diff>